<commit_message>
due dataframes in asingle sheet _ok
</commit_message>
<xml_diff>
--- a/conti_camerino_multiple.xlsx
+++ b/conti_camerino_multiple.xlsx
@@ -508,7 +508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,12 +534,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>gennaio</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>All</t>
+          <t>Euro</t>
         </is>
       </c>
     </row>
@@ -560,10 +555,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>70.87</v>
-      </c>
-      <c r="E2" t="n">
-        <v>70.87</v>
+        <v>141.73</v>
       </c>
     </row>
     <row r="3">
@@ -577,9 +569,6 @@
       <c r="D3" t="n">
         <v>38.56</v>
       </c>
-      <c r="E3" t="n">
-        <v>38.56</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n"/>
@@ -590,10 +579,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
-      </c>
-      <c r="E4" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -607,9 +593,6 @@
       <c r="D5" t="n">
         <v>55.4</v>
       </c>
-      <c r="E5" t="n">
-        <v>55.4</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n"/>
@@ -626,9 +609,6 @@
       <c r="D6" t="n">
         <v>50</v>
       </c>
-      <c r="E6" t="n">
-        <v>50</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
@@ -643,10 +623,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>274.33</v>
-      </c>
-      <c r="E7" t="n">
-        <v>274.33</v>
+        <v>823</v>
       </c>
     </row>
     <row r="8">
@@ -660,9 +637,6 @@
       <c r="D8" t="n">
         <v>630</v>
       </c>
-      <c r="E8" t="n">
-        <v>630</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
@@ -673,10 +647,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>75.18000000000001</v>
-      </c>
-      <c r="E9" t="n">
-        <v>75.18000000000001</v>
+        <v>150.36</v>
       </c>
     </row>
     <row r="10">
@@ -692,9 +663,6 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>100.32</v>
-      </c>
-      <c r="E10" t="n">
         <v>100.32</v>
       </c>
     </row>
@@ -709,9 +677,6 @@
       <c r="D11" t="n">
         <v>30</v>
       </c>
-      <c r="E11" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n"/>
@@ -728,9 +693,6 @@
       <c r="D12" t="n">
         <v>130</v>
       </c>
-      <c r="E12" t="n">
-        <v>130</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
@@ -747,9 +709,6 @@
       <c r="D13" t="n">
         <v>1185.57</v>
       </c>
-      <c r="E13" t="n">
-        <v>1185.57</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n"/>
@@ -764,10 +723,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>82.34999999999999</v>
-      </c>
-      <c r="E14" t="n">
-        <v>82.34999999999999</v>
+        <v>1070.56</v>
       </c>
     </row>
     <row r="15">
@@ -781,9 +737,6 @@
       <c r="D15" t="n">
         <v>4.5</v>
       </c>
-      <c r="E15" t="n">
-        <v>4.5</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n"/>
@@ -798,10 +751,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>33.82</v>
-      </c>
-      <c r="E16" t="n">
-        <v>33.82</v>
+        <v>135.26</v>
       </c>
     </row>
     <row r="17">
@@ -813,10 +763,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>6.88</v>
-      </c>
-      <c r="E17" t="n">
-        <v>6.88</v>
+        <v>13.75</v>
       </c>
     </row>
     <row r="18">
@@ -830,9 +777,6 @@
       <c r="D18" t="n">
         <v>5.5</v>
       </c>
-      <c r="E18" t="n">
-        <v>5.5</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n"/>
@@ -847,10 +791,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>22.68</v>
-      </c>
-      <c r="E19" t="n">
-        <v>22.68</v>
+        <v>113.4</v>
       </c>
     </row>
     <row r="20">
@@ -864,9 +805,6 @@
       <c r="D20" t="n">
         <v>116</v>
       </c>
-      <c r="E20" t="n">
-        <v>116</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n"/>
@@ -881,10 +819,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>35.98</v>
-      </c>
-      <c r="E21" t="n">
-        <v>35.98</v>
+        <v>71.95</v>
       </c>
     </row>
     <row r="22">
@@ -902,9 +837,6 @@
       <c r="D22" t="n">
         <v>10</v>
       </c>
-      <c r="E22" t="n">
-        <v>10</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n"/>
@@ -919,10 +851,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>121.78</v>
-      </c>
-      <c r="E23" t="n">
-        <v>121.78</v>
+        <v>243.56</v>
       </c>
     </row>
     <row r="24">
@@ -940,9 +869,6 @@
       <c r="D24" t="n">
         <v>24</v>
       </c>
-      <c r="E24" t="n">
-        <v>24</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n"/>
@@ -957,10 +883,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>108.51</v>
-      </c>
-      <c r="E25" t="n">
-        <v>108.51</v>
+        <v>542.5599999999999</v>
       </c>
     </row>
     <row r="26">
@@ -974,9 +897,6 @@
       <c r="D26" t="n">
         <v>533</v>
       </c>
-      <c r="E26" t="n">
-        <v>533</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n"/>
@@ -987,10 +907,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>86.09</v>
-      </c>
-      <c r="E27" t="n">
-        <v>86.09</v>
+        <v>344.36</v>
       </c>
     </row>
     <row r="28">
@@ -1002,10 +919,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>63.79</v>
-      </c>
-      <c r="E28" t="n">
-        <v>63.79</v>
+        <v>255.16</v>
       </c>
     </row>
     <row r="29">
@@ -1017,10 +931,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>45.5</v>
-      </c>
-      <c r="E29" t="n">
-        <v>45.5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30">
@@ -1034,9 +945,6 @@
       <c r="D30" t="n">
         <v>54.9</v>
       </c>
-      <c r="E30" t="n">
-        <v>54.9</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -1047,10 +955,7 @@
       <c r="B31" s="1" t="n"/>
       <c r="C31" s="1" t="n"/>
       <c r="D31" t="n">
-        <v>104.54</v>
-      </c>
-      <c r="E31" t="n">
-        <v>104.54</v>
+        <v>7004.4</v>
       </c>
     </row>
   </sheetData>
@@ -1074,7 +979,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1100,12 +1005,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>gennaio</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>All</t>
+          <t>Euro</t>
         </is>
       </c>
     </row>
@@ -1126,10 +1026,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>272</v>
-      </c>
-      <c r="E2" t="n">
-        <v>272</v>
+        <v>544</v>
       </c>
     </row>
     <row r="3">
@@ -1145,9 +1042,6 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1060.05</v>
-      </c>
-      <c r="E3" t="n">
         <v>1060.05</v>
       </c>
     </row>
@@ -1162,9 +1056,6 @@
       <c r="D4" t="n">
         <v>1028.81</v>
       </c>
-      <c r="E4" t="n">
-        <v>1028.81</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
@@ -1181,9 +1072,6 @@
       <c r="D5" t="n">
         <v>52.36</v>
       </c>
-      <c r="E5" t="n">
-        <v>52.36</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n"/>
@@ -1198,9 +1086,6 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>50</v>
-      </c>
-      <c r="E6" t="n">
         <v>50</v>
       </c>
     </row>
@@ -1213,10 +1098,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>394.29</v>
-      </c>
-      <c r="E7" t="n">
-        <v>394.29</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="8">
@@ -1228,10 +1110,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>128</v>
-      </c>
-      <c r="E8" t="n">
-        <v>128</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9">
@@ -1247,9 +1126,6 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>635</v>
-      </c>
-      <c r="E9" t="n">
         <v>635</v>
       </c>
     </row>
@@ -1264,9 +1140,6 @@
       <c r="D10" t="n">
         <v>635</v>
       </c>
-      <c r="E10" t="n">
-        <v>635</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
@@ -1279,9 +1152,6 @@
       <c r="D11" t="n">
         <v>635</v>
       </c>
-      <c r="E11" t="n">
-        <v>635</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n"/>
@@ -1294,9 +1164,6 @@
       <c r="D12" t="n">
         <v>635</v>
       </c>
-      <c r="E12" t="n">
-        <v>635</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
@@ -1311,10 +1178,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>28.36</v>
-      </c>
-      <c r="E13" t="n">
-        <v>28.36</v>
+        <v>226.89</v>
       </c>
     </row>
     <row r="14">
@@ -1328,9 +1192,6 @@
       <c r="D14" t="n">
         <v>6.2</v>
       </c>
-      <c r="E14" t="n">
-        <v>6.2</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n"/>
@@ -1345,10 +1206,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>200</v>
-      </c>
-      <c r="E15" t="n">
-        <v>200</v>
+        <v>600</v>
       </c>
     </row>
     <row r="16">
@@ -1360,10 +1218,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>132.5</v>
-      </c>
-      <c r="E16" t="n">
-        <v>132.5</v>
+        <v>530</v>
       </c>
     </row>
     <row r="17">
@@ -1379,10 +1234,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>20</v>
-      </c>
-      <c r="E17" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
@@ -1394,10 +1246,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>460</v>
-      </c>
-      <c r="E18" t="n">
-        <v>460</v>
+        <v>920</v>
       </c>
     </row>
     <row r="19">
@@ -1409,10 +1258,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>10</v>
-      </c>
-      <c r="E19" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20">
@@ -1424,10 +1270,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>54.42</v>
-      </c>
-      <c r="E20" t="n">
-        <v>54.42</v>
+        <v>326.5</v>
       </c>
     </row>
     <row r="21">
@@ -1439,10 +1282,7 @@
       <c r="B21" s="1" t="n"/>
       <c r="C21" s="1" t="n"/>
       <c r="D21" t="n">
-        <v>228.77</v>
-      </c>
-      <c r="E21" t="n">
-        <v>228.77</v>
+        <v>10980.81</v>
       </c>
     </row>
   </sheetData>
@@ -1465,7 +1305,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1491,12 +1331,7 @@
       </c>
       <c r="D1" s="4" t="inlineStr">
         <is>
-          <t>gennaio</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>All</t>
+          <t>Euro</t>
         </is>
       </c>
     </row>
@@ -1517,10 +1352,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>272</v>
-      </c>
-      <c r="E2" t="n">
-        <v>272</v>
+        <v>544</v>
       </c>
     </row>
     <row r="3">
@@ -1536,9 +1368,6 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1060.05</v>
-      </c>
-      <c r="E3" t="n">
         <v>1060.05</v>
       </c>
     </row>
@@ -1553,9 +1382,6 @@
       <c r="D4" t="n">
         <v>1028.81</v>
       </c>
-      <c r="E4" t="n">
-        <v>1028.81</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="n"/>
@@ -1572,9 +1398,6 @@
       <c r="D5" t="n">
         <v>52.36</v>
       </c>
-      <c r="E5" t="n">
-        <v>52.36</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="n"/>
@@ -1589,9 +1412,6 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>50</v>
-      </c>
-      <c r="E6" t="n">
         <v>50</v>
       </c>
     </row>
@@ -1604,10 +1424,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>394.29</v>
-      </c>
-      <c r="E7" t="n">
-        <v>394.29</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="8">
@@ -1619,10 +1436,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>128</v>
-      </c>
-      <c r="E8" t="n">
-        <v>128</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9">
@@ -1638,9 +1452,6 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>635</v>
-      </c>
-      <c r="E9" t="n">
         <v>635</v>
       </c>
     </row>
@@ -1655,9 +1466,6 @@
       <c r="D10" t="n">
         <v>635</v>
       </c>
-      <c r="E10" t="n">
-        <v>635</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="n"/>
@@ -1670,9 +1478,6 @@
       <c r="D11" t="n">
         <v>635</v>
       </c>
-      <c r="E11" t="n">
-        <v>635</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="n"/>
@@ -1685,9 +1490,6 @@
       <c r="D12" t="n">
         <v>635</v>
       </c>
-      <c r="E12" t="n">
-        <v>635</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="n"/>
@@ -1702,10 +1504,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>28.36</v>
-      </c>
-      <c r="E13" t="n">
-        <v>28.36</v>
+        <v>226.89</v>
       </c>
     </row>
     <row r="14">
@@ -1719,9 +1518,6 @@
       <c r="D14" t="n">
         <v>6.2</v>
       </c>
-      <c r="E14" t="n">
-        <v>6.2</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="n"/>
@@ -1736,10 +1532,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>200</v>
-      </c>
-      <c r="E15" t="n">
-        <v>200</v>
+        <v>600</v>
       </c>
     </row>
     <row r="16">
@@ -1751,10 +1544,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>132.5</v>
-      </c>
-      <c r="E16" t="n">
-        <v>132.5</v>
+        <v>530</v>
       </c>
     </row>
     <row r="17">
@@ -1770,10 +1560,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>20</v>
-      </c>
-      <c r="E17" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
@@ -1785,10 +1572,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>460</v>
-      </c>
-      <c r="E18" t="n">
-        <v>460</v>
+        <v>920</v>
       </c>
     </row>
     <row r="19">
@@ -1800,10 +1584,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>10</v>
-      </c>
-      <c r="E19" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20">
@@ -1815,10 +1596,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>54.42</v>
-      </c>
-      <c r="E20" t="n">
-        <v>54.42</v>
+        <v>326.5</v>
       </c>
     </row>
     <row r="21">
@@ -1830,10 +1608,7 @@
       <c r="B21" s="4" t="inlineStr"/>
       <c r="C21" s="4" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>228.77</v>
-      </c>
-      <c r="E21" t="n">
-        <v>228.77</v>
+        <v>10980.81</v>
       </c>
     </row>
     <row r="26">
@@ -1854,12 +1629,7 @@
       </c>
       <c r="D26" s="4" t="inlineStr">
         <is>
-          <t>gennaio</t>
-        </is>
-      </c>
-      <c r="E26" s="4" t="inlineStr">
-        <is>
-          <t>All</t>
+          <t>Euro</t>
         </is>
       </c>
     </row>
@@ -1880,10 +1650,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>70.87</v>
-      </c>
-      <c r="E27" t="n">
-        <v>70.87</v>
+        <v>141.73</v>
       </c>
     </row>
     <row r="28">
@@ -1897,9 +1664,6 @@
       <c r="D28" t="n">
         <v>38.56</v>
       </c>
-      <c r="E28" t="n">
-        <v>38.56</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="n"/>
@@ -1910,10 +1674,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>20</v>
-      </c>
-      <c r="E29" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30">
@@ -1927,9 +1688,6 @@
       <c r="D30" t="n">
         <v>55.4</v>
       </c>
-      <c r="E30" t="n">
-        <v>55.4</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="n"/>
@@ -1946,9 +1704,6 @@
       <c r="D31" t="n">
         <v>50</v>
       </c>
-      <c r="E31" t="n">
-        <v>50</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="n"/>
@@ -1963,10 +1718,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>274.33</v>
-      </c>
-      <c r="E32" t="n">
-        <v>274.33</v>
+        <v>823</v>
       </c>
     </row>
     <row r="33">
@@ -1980,9 +1732,6 @@
       <c r="D33" t="n">
         <v>630</v>
       </c>
-      <c r="E33" t="n">
-        <v>630</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="n"/>
@@ -1993,10 +1742,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>75.18000000000001</v>
-      </c>
-      <c r="E34" t="n">
-        <v>75.18000000000001</v>
+        <v>150.36</v>
       </c>
     </row>
     <row r="35">
@@ -2012,9 +1758,6 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>100.32</v>
-      </c>
-      <c r="E35" t="n">
         <v>100.32</v>
       </c>
     </row>
@@ -2029,9 +1772,6 @@
       <c r="D36" t="n">
         <v>30</v>
       </c>
-      <c r="E36" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" s="4" t="n"/>
@@ -2048,9 +1788,6 @@
       <c r="D37" t="n">
         <v>130</v>
       </c>
-      <c r="E37" t="n">
-        <v>130</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="n"/>
@@ -2067,9 +1804,6 @@
       <c r="D38" t="n">
         <v>1185.57</v>
       </c>
-      <c r="E38" t="n">
-        <v>1185.57</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="n"/>
@@ -2084,10 +1818,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>82.34999999999999</v>
-      </c>
-      <c r="E39" t="n">
-        <v>82.34999999999999</v>
+        <v>1070.56</v>
       </c>
     </row>
     <row r="40">
@@ -2101,9 +1832,6 @@
       <c r="D40" t="n">
         <v>4.5</v>
       </c>
-      <c r="E40" t="n">
-        <v>4.5</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" s="4" t="n"/>
@@ -2118,10 +1846,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>33.82</v>
-      </c>
-      <c r="E41" t="n">
-        <v>33.82</v>
+        <v>135.26</v>
       </c>
     </row>
     <row r="42">
@@ -2133,10 +1858,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>6.88</v>
-      </c>
-      <c r="E42" t="n">
-        <v>6.88</v>
+        <v>13.75</v>
       </c>
     </row>
     <row r="43">
@@ -2150,9 +1872,6 @@
       <c r="D43" t="n">
         <v>5.5</v>
       </c>
-      <c r="E43" t="n">
-        <v>5.5</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" s="4" t="n"/>
@@ -2167,10 +1886,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>22.68</v>
-      </c>
-      <c r="E44" t="n">
-        <v>22.68</v>
+        <v>113.4</v>
       </c>
     </row>
     <row r="45">
@@ -2184,9 +1900,6 @@
       <c r="D45" t="n">
         <v>116</v>
       </c>
-      <c r="E45" t="n">
-        <v>116</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" s="4" t="n"/>
@@ -2201,10 +1914,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>35.98</v>
-      </c>
-      <c r="E46" t="n">
-        <v>35.98</v>
+        <v>71.95</v>
       </c>
     </row>
     <row r="47">
@@ -2222,9 +1932,6 @@
       <c r="D47" t="n">
         <v>10</v>
       </c>
-      <c r="E47" t="n">
-        <v>10</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" s="4" t="n"/>
@@ -2239,10 +1946,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>121.78</v>
-      </c>
-      <c r="E48" t="n">
-        <v>121.78</v>
+        <v>243.56</v>
       </c>
     </row>
     <row r="49">
@@ -2260,9 +1964,6 @@
       <c r="D49" t="n">
         <v>24</v>
       </c>
-      <c r="E49" t="n">
-        <v>24</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" s="4" t="n"/>
@@ -2277,10 +1978,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>108.51</v>
-      </c>
-      <c r="E50" t="n">
-        <v>108.51</v>
+        <v>542.5599999999999</v>
       </c>
     </row>
     <row r="51">
@@ -2294,9 +1992,6 @@
       <c r="D51" t="n">
         <v>533</v>
       </c>
-      <c r="E51" t="n">
-        <v>533</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" s="4" t="n"/>
@@ -2307,10 +2002,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>86.09</v>
-      </c>
-      <c r="E52" t="n">
-        <v>86.09</v>
+        <v>344.36</v>
       </c>
     </row>
     <row r="53">
@@ -2322,10 +2014,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>63.79</v>
-      </c>
-      <c r="E53" t="n">
-        <v>63.79</v>
+        <v>255.16</v>
       </c>
     </row>
     <row r="54">
@@ -2337,10 +2026,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>45.5</v>
-      </c>
-      <c r="E54" t="n">
-        <v>45.5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55">
@@ -2354,9 +2040,6 @@
       <c r="D55" t="n">
         <v>54.9</v>
       </c>
-      <c r="E55" t="n">
-        <v>54.9</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" s="4" t="inlineStr">
@@ -2367,10 +2050,7 @@
       <c r="B56" s="4" t="inlineStr"/>
       <c r="C56" s="4" t="inlineStr"/>
       <c r="D56" t="n">
-        <v>104.54</v>
-      </c>
-      <c r="E56" t="n">
-        <v>104.54</v>
+        <v>7004.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>